<commit_message>
Edit formatted excel file
</commit_message>
<xml_diff>
--- a/bliblinventory/format-tambah-barang-bulk.xlsx
+++ b/bliblinventory/format-tambah-barang-bulk.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Desktop\Bliblinventory2.0\bliblinventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C3D531-04C5-4296-8DA0-52F81249188C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5743A902-CEE3-486C-AA96-56E27A34D73A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{01CC1072-85B4-4092-8C1B-B5B45CCA280E}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>KODE</t>
   </si>
@@ -59,30 +59,6 @@
   </si>
   <si>
     <t>NAMA FILE GAMBAR</t>
-  </si>
-  <si>
-    <t>LTP0002</t>
-  </si>
-  <si>
-    <t>LAPTOP ACER SWIFT 3</t>
-  </si>
-  <si>
-    <t>INI LAPTOP ACER BUKAN ASUS</t>
-  </si>
-  <si>
-    <t>acer-swift-3.jpg</t>
-  </si>
-  <si>
-    <t>LTP0003</t>
-  </si>
-  <si>
-    <t>LAPTOP ASUS ROG</t>
-  </si>
-  <si>
-    <t>INI LAPTOP GAMING</t>
-  </si>
-  <si>
-    <t>asus-rog.jpg</t>
   </si>
 </sst>
 </file>
@@ -444,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AAC6D15-B71A-4E24-9646-D8C195F2828C}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="G3" sqref="A2:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,52 +457,6 @@
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="2">
-        <v>8000000</v>
-      </c>
-      <c r="G2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="2">
-        <v>15000000</v>
-      </c>
-      <c r="G3" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>